<commit_message>
remove patients without C-ids
</commit_message>
<xml_diff>
--- a/analyses/11-tables/output/Table-S1.xlsx
+++ b/analyses/11-tables/output/Table-S1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
   <si>
     <t xml:space="preserve">Patient ID</t>
   </si>
@@ -438,21 +438,6 @@
   </si>
   <si>
     <t xml:space="preserve">7316-466</t>
-  </si>
-  <si>
-    <t xml:space="preserve">795-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">795-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">795-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">795-70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">795-72</t>
   </si>
 </sst>
 </file>
@@ -2448,136 +2433,6 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B65" t="s">
-        <v>142</v>
-      </c>
-      <c r="C65" t="s">
-        <v>22</v>
-      </c>
-      <c r="D65" t="s">
-        <v>17</v>
-      </c>
-      <c r="E65" t="s">
-        <v>12</v>
-      </c>
-      <c r="F65" t="s">
-        <v>13</v>
-      </c>
-      <c r="G65" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H65" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B66" t="s">
-        <v>143</v>
-      </c>
-      <c r="C66" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66" t="s">
-        <v>17</v>
-      </c>
-      <c r="E66" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66" t="s">
-        <v>13</v>
-      </c>
-      <c r="G66" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H66" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B67" t="s">
-        <v>144</v>
-      </c>
-      <c r="C67" t="s">
-        <v>22</v>
-      </c>
-      <c r="D67" t="s">
-        <v>17</v>
-      </c>
-      <c r="E67" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" t="s">
-        <v>18</v>
-      </c>
-      <c r="G67" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H67" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B68" t="s">
-        <v>145</v>
-      </c>
-      <c r="C68" t="s">
-        <v>22</v>
-      </c>
-      <c r="D68" t="s">
-        <v>17</v>
-      </c>
-      <c r="E68" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" t="s">
-        <v>18</v>
-      </c>
-      <c r="G68" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H68" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B69" t="s">
-        <v>146</v>
-      </c>
-      <c r="C69" t="s">
-        <v>22</v>
-      </c>
-      <c r="D69" t="s">
-        <v>17</v>
-      </c>
-      <c r="E69" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" t="s">
-        <v>18</v>
-      </c>
-      <c r="G69" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H69" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
add oncogenic DGD ATRX mut to Table S1
</commit_message>
<xml_diff>
--- a/analyses/11-tables/output/Table-S1.xlsx
+++ b/analyses/11-tables/output/Table-S1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
   <si>
     <t xml:space="preserve">Patient ID</t>
   </si>
@@ -92,9 +92,6 @@
     <t xml:space="preserve">Not Reported</t>
   </si>
   <si>
-    <t xml:space="preserve">Not profiled</t>
-  </si>
-  <si>
     <t xml:space="preserve">C1064934</t>
   </si>
   <si>
@@ -128,13 +125,7 @@
     <t xml:space="preserve">7316-4723</t>
   </si>
   <si>
-    <t xml:space="preserve">p.S930Ffs*7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p.E929Qfs*8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p.E929Q</t>
+    <t xml:space="preserve">p.S930Ffs*7, p.E929Qfs*8</t>
   </si>
   <si>
     <t xml:space="preserve">C1190886</t>
@@ -155,7 +146,7 @@
     <t xml:space="preserve">7316-4917</t>
   </si>
   <si>
-    <t xml:space="preserve">p.R1803H</t>
+    <t xml:space="preserve">p.R1803H (VUS)</t>
   </si>
   <si>
     <t xml:space="preserve">C15990</t>
@@ -221,9 +212,6 @@
     <t xml:space="preserve">p.E1757*</t>
   </si>
   <si>
-    <t xml:space="preserve">p.H865Q</t>
-  </si>
-  <si>
     <t xml:space="preserve">C2356434</t>
   </si>
   <si>
@@ -239,12 +227,12 @@
     <t xml:space="preserve">C271092</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2146</t>
+  </si>
+  <si>
     <t xml:space="preserve">7316-2751</t>
   </si>
   <si>
-    <t xml:space="preserve">7316-2146</t>
-  </si>
-  <si>
     <t xml:space="preserve">C27306</t>
   </si>
   <si>
@@ -404,7 +392,7 @@
     <t xml:space="preserve">7316-3058</t>
   </si>
   <si>
-    <t xml:space="preserve">p.R2197C</t>
+    <t xml:space="preserve">p.R2197C (VUS)</t>
   </si>
   <si>
     <t xml:space="preserve">C744765</t>
@@ -425,7 +413,7 @@
     <t xml:space="preserve">7316-3027</t>
   </si>
   <si>
-    <t xml:space="preserve">p.N1441K</t>
+    <t xml:space="preserve">p.N1441K (VUS)</t>
   </si>
   <si>
     <t xml:space="preserve">C806142</t>
@@ -949,8 +937,8 @@
       <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
-        <v>26</v>
+      <c r="G5" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H5" t="e">
         <v>#N/A</v>
@@ -961,10 +949,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -990,13 +978,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
@@ -1019,10 +1007,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -1036,8 +1024,8 @@
       <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
-        <v>26</v>
+      <c r="G8" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H8" t="e">
         <v>#N/A</v>
@@ -1048,10 +1036,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -1065,8 +1053,8 @@
       <c r="F9" t="s">
         <v>20</v>
       </c>
-      <c r="G9" t="s">
-        <v>26</v>
+      <c r="G9" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H9" t="e">
         <v>#N/A</v>
@@ -1077,10 +1065,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1095,7 +1083,7 @@
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" t="e">
         <v>#N/A</v>
@@ -1106,25 +1094,25 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="H11" t="e">
         <v>#N/A</v>
@@ -1135,25 +1123,25 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="H12" t="e">
         <v>#N/A</v>
@@ -1164,16 +1152,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -1182,7 +1170,7 @@
         <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H13" t="e">
         <v>#N/A</v>
@@ -1193,25 +1181,25 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
       </c>
-      <c r="G14" t="s">
-        <v>21</v>
+      <c r="G14" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H14" t="e">
         <v>#N/A</v>
@@ -1222,100 +1210,100 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.55</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.989</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="H17" t="n">
-        <v>0.55</v>
+        <v>1.198</v>
       </c>
       <c r="I17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -1326,55 +1314,55 @@
       <c r="F18" t="s">
         <v>20</v>
       </c>
-      <c r="G18" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.989</v>
+      <c r="G18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H18" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I18" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
         <v>20</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="H19" t="n">
-        <v>1.198</v>
+        <v>0.929</v>
       </c>
       <c r="I19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
         <v>60</v>
       </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
       <c r="D20" t="s">
         <v>12</v>
       </c>
@@ -1384,8 +1372,8 @@
       <c r="F20" t="s">
         <v>20</v>
       </c>
-      <c r="G20" t="s">
-        <v>26</v>
+      <c r="G20" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H20" t="e">
         <v>#N/A</v>
@@ -1396,54 +1384,54 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.929</v>
+        <v>65</v>
+      </c>
+      <c r="H21" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I21" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H22" t="e">
         <v>#N/A</v>
@@ -1454,57 +1442,57 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
-      </c>
-      <c r="H23" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.896</v>
       </c>
       <c r="I23" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
-      </c>
-      <c r="H24" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.765</v>
       </c>
       <c r="I24" t="s">
         <v>16</v>
@@ -1515,16 +1503,16 @@
         <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
         <v>20</v>
@@ -1532,51 +1520,51 @@
       <c r="G25" t="s">
         <v>21</v>
       </c>
-      <c r="H25" t="e">
-        <v>#N/A</v>
+      <c r="H25" t="n">
+        <v>0.578</v>
       </c>
       <c r="I25" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="H26" t="n">
-        <v>0.896</v>
+        <v>1.905</v>
       </c>
       <c r="I26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -1591,27 +1579,27 @@
         <v>21</v>
       </c>
       <c r="H27" t="n">
-        <v>0.578</v>
+        <v>0.785</v>
       </c>
       <c r="I27" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
         <v>20</v>
@@ -1620,18 +1608,18 @@
         <v>21</v>
       </c>
       <c r="H28" t="n">
-        <v>0.765</v>
+        <v>3.437</v>
       </c>
       <c r="I28" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
@@ -1643,24 +1631,24 @@
         <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G29" t="s">
-        <v>79</v>
-      </c>
-      <c r="H29" t="n">
-        <v>1.905</v>
+        <v>21</v>
+      </c>
+      <c r="H29" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I29" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
@@ -1678,56 +1666,56 @@
         <v>21</v>
       </c>
       <c r="H30" t="n">
-        <v>0.785</v>
+        <v>0.724</v>
       </c>
       <c r="I30" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
         <v>20</v>
       </c>
-      <c r="G31" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" t="n">
-        <v>3.437</v>
+      <c r="G31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H31" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I31" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" t="s">
         <v>20</v>
@@ -1735,54 +1723,54 @@
       <c r="G32" t="s">
         <v>21</v>
       </c>
-      <c r="H32" t="e">
-        <v>#N/A</v>
+      <c r="H32" t="n">
+        <v>0.883</v>
       </c>
       <c r="I32" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F33" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G33" t="s">
         <v>21</v>
       </c>
       <c r="H33" t="n">
-        <v>0.724</v>
+        <v>2.78</v>
       </c>
       <c r="I33" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1791,21 +1779,21 @@
         <v>20</v>
       </c>
       <c r="G34" t="s">
-        <v>26</v>
-      </c>
-      <c r="H34" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.665</v>
       </c>
       <c r="I34" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -1823,21 +1811,21 @@
         <v>21</v>
       </c>
       <c r="H35" t="n">
-        <v>0.883</v>
+        <v>1.155</v>
       </c>
       <c r="I35" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D36" t="s">
         <v>13</v>
@@ -1848,28 +1836,28 @@
       <c r="F36" t="s">
         <v>14</v>
       </c>
-      <c r="G36" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" t="n">
-        <v>2.78</v>
+      <c r="G36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I36" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -1877,54 +1865,54 @@
       <c r="F37" t="s">
         <v>20</v>
       </c>
-      <c r="G37" t="s">
-        <v>21</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0.665</v>
+      <c r="G37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H37" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I37" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G38" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="H38" t="n">
-        <v>1.155</v>
+        <v>4.859</v>
       </c>
       <c r="I38" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
@@ -1936,53 +1924,53 @@
         <v>14</v>
       </c>
       <c r="G39" t="s">
-        <v>26</v>
-      </c>
-      <c r="H39" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1.077</v>
       </c>
       <c r="I39" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F40" t="s">
         <v>20</v>
       </c>
       <c r="G40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H40" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="H40" t="n">
+        <v>8.822</v>
       </c>
       <c r="I40" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
@@ -1991,45 +1979,45 @@
         <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G41" t="s">
-        <v>104</v>
+        <v>21</v>
       </c>
       <c r="H41" t="n">
-        <v>4.859</v>
+        <v>4.079</v>
       </c>
       <c r="I41" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B42" t="s">
         <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" t="s">
-        <v>21</v>
-      </c>
-      <c r="H42" t="n">
-        <v>1.077</v>
+        <v>20</v>
+      </c>
+      <c r="G42" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H42" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I42" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43">
@@ -2040,51 +2028,51 @@
         <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D43" t="s">
         <v>13</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43" t="s">
-        <v>21</v>
-      </c>
-      <c r="H43" t="n">
-        <v>8.822</v>
+        <v>14</v>
+      </c>
+      <c r="G43" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H43" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I43" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C44" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D44" t="s">
         <v>13</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F44" t="s">
-        <v>19</v>
-      </c>
-      <c r="G44" t="s">
-        <v>21</v>
-      </c>
-      <c r="H44" t="n">
-        <v>4.079</v>
+        <v>20</v>
+      </c>
+      <c r="G44" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H44" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I44" t="s">
         <v>16</v>
@@ -2092,25 +2080,25 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
         <v>25</v>
       </c>
       <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
         <v>19</v>
       </c>
-      <c r="E45" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" t="s">
-        <v>20</v>
-      </c>
-      <c r="G45" t="s">
-        <v>26</v>
+      <c r="G45" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H45" t="e">
         <v>#N/A</v>
@@ -2121,45 +2109,45 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E46" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G46" t="s">
-        <v>26</v>
-      </c>
-      <c r="H46" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.662</v>
       </c>
       <c r="I46" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
         <v>11</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -2168,24 +2156,24 @@
         <v>20</v>
       </c>
       <c r="G47" t="s">
-        <v>26</v>
-      </c>
-      <c r="H47" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.911</v>
       </c>
       <c r="I47" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C48" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
@@ -2194,56 +2182,56 @@
         <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G48" t="s">
-        <v>26</v>
-      </c>
-      <c r="H48" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.768</v>
       </c>
       <c r="I48" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D49" t="s">
         <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F49" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G49" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H49" t="n">
-        <v>0.662</v>
+        <v>1.494</v>
       </c>
       <c r="I49" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
@@ -2252,85 +2240,85 @@
         <v>12</v>
       </c>
       <c r="F50" t="s">
-        <v>20</v>
-      </c>
-      <c r="G50" t="s">
-        <v>21</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0.911</v>
+        <v>14</v>
+      </c>
+      <c r="G50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H50" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I50" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B51" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D51" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F51" t="s">
         <v>20</v>
       </c>
       <c r="G51" t="s">
-        <v>21</v>
+        <v>126</v>
       </c>
       <c r="H51" t="n">
-        <v>0.768</v>
+        <v>1.728</v>
       </c>
       <c r="I51" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B52" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
       <c r="E52" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F52" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G52" t="s">
-        <v>125</v>
+        <v>21</v>
       </c>
       <c r="H52" t="n">
-        <v>1.494</v>
+        <v>0.954</v>
       </c>
       <c r="I52" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>
@@ -2339,42 +2327,42 @@
         <v>12</v>
       </c>
       <c r="F53" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G53" t="s">
-        <v>26</v>
-      </c>
-      <c r="H53" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.453</v>
       </c>
       <c r="I53" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B54" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C54" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D54" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F54" t="s">
         <v>20</v>
       </c>
       <c r="G54" t="s">
-        <v>130</v>
-      </c>
-      <c r="H54" t="n">
-        <v>1.728</v>
+        <v>133</v>
+      </c>
+      <c r="H54" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I54" t="s">
         <v>16</v>
@@ -2382,48 +2370,48 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B55" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C55" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
       </c>
       <c r="E55" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F55" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G55" t="s">
         <v>21</v>
       </c>
       <c r="H55" t="n">
-        <v>0.954</v>
+        <v>0.409</v>
       </c>
       <c r="I55" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B56" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E56" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F56" t="s">
         <v>20</v>
@@ -2432,56 +2420,56 @@
         <v>21</v>
       </c>
       <c r="H56" t="n">
-        <v>0.453</v>
+        <v>4.471</v>
       </c>
       <c r="I56" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B57" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C57" t="s">
         <v>11</v>
       </c>
       <c r="D57" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E57" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G57" t="s">
-        <v>137</v>
-      </c>
-      <c r="H57" t="e">
-        <v>#N/A</v>
+        <v>140</v>
+      </c>
+      <c r="H57" t="n">
+        <v>1.733</v>
       </c>
       <c r="I57" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B58" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E58" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F58" t="s">
         <v>20</v>
@@ -2490,21 +2478,21 @@
         <v>21</v>
       </c>
       <c r="H58" t="n">
-        <v>0.409</v>
+        <v>5.205</v>
       </c>
       <c r="I58" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B59" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C59" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D59" t="s">
         <v>13</v>
@@ -2519,56 +2507,56 @@
         <v>21</v>
       </c>
       <c r="H59" t="n">
-        <v>4.471</v>
+        <v>10.845</v>
       </c>
       <c r="I59" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B60" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C60" t="s">
         <v>11</v>
       </c>
       <c r="D60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F60" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G60" t="s">
-        <v>144</v>
+        <v>21</v>
       </c>
       <c r="H60" t="n">
-        <v>1.733</v>
+        <v>0.953</v>
       </c>
       <c r="I60" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B61" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C61" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="D61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F61" t="s">
         <v>20</v>
@@ -2577,27 +2565,27 @@
         <v>21</v>
       </c>
       <c r="H61" t="n">
-        <v>5.205</v>
+        <v>0.408</v>
       </c>
       <c r="I61" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B62" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C62" t="s">
         <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F62" t="s">
         <v>20</v>
@@ -2606,18 +2594,18 @@
         <v>21</v>
       </c>
       <c r="H62" t="n">
-        <v>10.845</v>
+        <v>1.025</v>
       </c>
       <c r="I62" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C63" t="s">
         <v>11</v>
@@ -2635,97 +2623,10 @@
         <v>21</v>
       </c>
       <c r="H63" t="n">
-        <v>0.953</v>
+        <v>0.391</v>
       </c>
       <c r="I63" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>151</v>
-      </c>
-      <c r="B64" t="s">
-        <v>152</v>
-      </c>
-      <c r="C64" t="s">
-        <v>31</v>
-      </c>
-      <c r="D64" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64" t="s">
-        <v>12</v>
-      </c>
-      <c r="F64" t="s">
-        <v>20</v>
-      </c>
-      <c r="G64" t="s">
-        <v>21</v>
-      </c>
-      <c r="H64" t="n">
-        <v>0.408</v>
-      </c>
-      <c r="I64" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>153</v>
-      </c>
-      <c r="B65" t="s">
-        <v>154</v>
-      </c>
-      <c r="C65" t="s">
-        <v>11</v>
-      </c>
-      <c r="D65" t="s">
-        <v>12</v>
-      </c>
-      <c r="E65" t="s">
-        <v>12</v>
-      </c>
-      <c r="F65" t="s">
-        <v>20</v>
-      </c>
-      <c r="G65" t="s">
-        <v>21</v>
-      </c>
-      <c r="H65" t="n">
-        <v>1.025</v>
-      </c>
-      <c r="I65" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>155</v>
-      </c>
-      <c r="B66" t="s">
-        <v>156</v>
-      </c>
-      <c r="C66" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66" t="s">
-        <v>12</v>
-      </c>
-      <c r="E66" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66" t="s">
-        <v>20</v>
-      </c>
-      <c r="G66" t="s">
-        <v>21</v>
-      </c>
-      <c r="H66" t="n">
-        <v>0.391</v>
-      </c>
-      <c r="I66" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move arrange to end
</commit_message>
<xml_diff>
--- a/analyses/11-tables/output/Table-S1.xlsx
+++ b/analyses/11-tables/output/Table-S1.xlsx
@@ -227,10 +227,10 @@
     <t xml:space="preserve">C271092</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2751</t>
+  </si>
+  <si>
     <t xml:space="preserve">7316-2146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7316-2751</t>
   </si>
   <si>
     <t xml:space="preserve">C27306</t>
@@ -1492,10 +1492,10 @@
         <v>21</v>
       </c>
       <c r="H24" t="n">
-        <v>0.765</v>
+        <v>0.578</v>
       </c>
       <c r="I24" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25">
@@ -1521,10 +1521,10 @@
         <v>21</v>
       </c>
       <c r="H25" t="n">
-        <v>0.578</v>
+        <v>0.765</v>
       </c>
       <c r="I25" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26">

</xml_diff>

<commit_message>
add CNV/SNVs to table S1
</commit_message>
<xml_diff>
--- a/analyses/11-tables/output/Table-S1.xlsx
+++ b/analyses/11-tables/output/Table-S1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t xml:space="preserve">Patient ID</t>
   </si>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">ATRX IHC</t>
   </si>
   <si>
-    <t xml:space="preserve">ATRXm</t>
+    <t xml:space="preserve">Somatic ATRX</t>
   </si>
   <si>
     <t xml:space="preserve">T/N TelHunt ratio</t>
@@ -284,6 +284,9 @@
     <t xml:space="preserve">7316-158</t>
   </si>
   <si>
+    <t xml:space="preserve">exon 1 DEL (promoter)</t>
+  </si>
+  <si>
     <t xml:space="preserve">C377610</t>
   </si>
   <si>
@@ -321,6 +324,9 @@
   </si>
   <si>
     <t xml:space="preserve">7316-2152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deep DEL (truncation)</t>
   </si>
   <si>
     <t xml:space="preserve">C53013</t>
@@ -1750,7 +1756,7 @@
         <v>14</v>
       </c>
       <c r="G33" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="H33" t="n">
         <v>2.78</v>
@@ -1761,10 +1767,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s">
         <v>30</v>
@@ -1790,10 +1796,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -1819,10 +1825,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C36" t="s">
         <v>30</v>
@@ -1848,10 +1854,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
@@ -1877,10 +1883,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
         <v>30</v>
@@ -1895,7 +1901,7 @@
         <v>14</v>
       </c>
       <c r="G38" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H38" t="n">
         <v>4.859</v>
@@ -1906,10 +1912,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
         <v>11</v>
@@ -1924,7 +1930,7 @@
         <v>14</v>
       </c>
       <c r="G39" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="H39" t="n">
         <v>1.077</v>
@@ -1935,10 +1941,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
         <v>30</v>
@@ -1964,10 +1970,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C41" t="s">
         <v>30</v>
@@ -1993,10 +1999,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
@@ -2022,10 +2028,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
@@ -2051,10 +2057,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
@@ -2080,10 +2086,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
         <v>25</v>
@@ -2109,10 +2115,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
@@ -2138,10 +2144,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C47" t="s">
         <v>11</v>
@@ -2167,10 +2173,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B48" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
@@ -2196,10 +2202,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C49" t="s">
         <v>30</v>
@@ -2214,7 +2220,7 @@
         <v>14</v>
       </c>
       <c r="G49" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H49" t="n">
         <v>1.494</v>
@@ -2225,10 +2231,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C50" t="s">
         <v>30</v>
@@ -2254,10 +2260,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C51" t="s">
         <v>30</v>
@@ -2272,7 +2278,7 @@
         <v>20</v>
       </c>
       <c r="G51" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H51" t="n">
         <v>1.728</v>
@@ -2283,10 +2289,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C52" t="s">
         <v>30</v>
@@ -2312,10 +2318,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B53" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C53" t="s">
         <v>30</v>
@@ -2341,10 +2347,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
         <v>11</v>
@@ -2359,7 +2365,7 @@
         <v>20</v>
       </c>
       <c r="G54" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H54" t="e">
         <v>#N/A</v>
@@ -2370,10 +2376,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C55" t="s">
         <v>11</v>
@@ -2399,10 +2405,10 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s">
         <v>30</v>
@@ -2428,10 +2434,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B57" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C57" t="s">
         <v>11</v>
@@ -2446,7 +2452,7 @@
         <v>14</v>
       </c>
       <c r="G57" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H57" t="n">
         <v>1.733</v>
@@ -2457,10 +2463,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B58" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C58" t="s">
         <v>52</v>
@@ -2486,10 +2492,10 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B59" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C59" t="s">
         <v>11</v>
@@ -2515,10 +2521,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B60" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C60" t="s">
         <v>11</v>
@@ -2544,10 +2550,10 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B61" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C61" t="s">
         <v>30</v>
@@ -2573,10 +2579,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B62" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C62" t="s">
         <v>11</v>
@@ -2602,10 +2608,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B63" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C63" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
add extra DGD samples
</commit_message>
<xml_diff>
--- a/analyses/11-tables/output/Table-S1.xlsx
+++ b/analyses/11-tables/output/Table-S1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t xml:space="preserve">Patient ID</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">7316-4678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.S1153*</t>
   </si>
   <si>
     <t xml:space="preserve">C115005</t>
@@ -943,8 +946,8 @@
       <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="e">
-        <v>#N/A</v>
+      <c r="G5" t="s">
+        <v>21</v>
       </c>
       <c r="H5" t="e">
         <v>#N/A</v>
@@ -1030,8 +1033,8 @@
       <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="G8" t="e">
-        <v>#N/A</v>
+      <c r="G8" t="s">
+        <v>33</v>
       </c>
       <c r="H8" t="e">
         <v>#N/A</v>
@@ -1042,10 +1045,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -1071,10 +1074,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1089,7 +1092,7 @@
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H10" t="e">
         <v>#N/A</v>
@@ -1100,10 +1103,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -1129,10 +1132,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
@@ -1158,10 +1161,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1176,7 +1179,7 @@
         <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H13" t="e">
         <v>#N/A</v>
@@ -1187,10 +1190,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1216,10 +1219,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -1240,18 +1243,18 @@
         <v>0.55</v>
       </c>
       <c r="I15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -1269,18 +1272,18 @@
         <v>0.989</v>
       </c>
       <c r="I16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
         <v>53</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -1292,21 +1295,21 @@
         <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H17" t="n">
         <v>1.198</v>
       </c>
       <c r="I17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>30</v>
@@ -1332,13 +1335,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -1356,18 +1359,18 @@
         <v>0.929</v>
       </c>
       <c r="I19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
         <v>61</v>
-      </c>
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -1390,10 +1393,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
         <v>30</v>
@@ -1408,7 +1411,7 @@
         <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H21" t="e">
         <v>#N/A</v>
@@ -1419,10 +1422,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1448,10 +1451,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
@@ -1472,15 +1475,15 @@
         <v>0.896</v>
       </c>
       <c r="I23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
         <v>30</v>
@@ -1501,15 +1504,15 @@
         <v>0.578</v>
       </c>
       <c r="I24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
@@ -1535,10 +1538,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1553,21 +1556,21 @@
         <v>14</v>
       </c>
       <c r="G26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H26" t="n">
         <v>1.905</v>
       </c>
       <c r="I26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
@@ -1588,18 +1591,18 @@
         <v>0.785</v>
       </c>
       <c r="I27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D28" t="s">
         <v>13</v>
@@ -1617,15 +1620,15 @@
         <v>3.437</v>
       </c>
       <c r="I28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
@@ -1651,10 +1654,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
@@ -1675,15 +1678,15 @@
         <v>0.724</v>
       </c>
       <c r="I30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
         <v>25</v>
@@ -1709,10 +1712,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
@@ -1733,15 +1736,15 @@
         <v>0.883</v>
       </c>
       <c r="I32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -1756,21 +1759,21 @@
         <v>14</v>
       </c>
       <c r="G33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H33" t="n">
         <v>2.78</v>
       </c>
       <c r="I33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
         <v>30</v>
@@ -1791,15 +1794,15 @@
         <v>0.665</v>
       </c>
       <c r="I34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -1820,15 +1823,15 @@
         <v>1.155</v>
       </c>
       <c r="I35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
         <v>30</v>
@@ -1854,10 +1857,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
@@ -1883,10 +1886,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C38" t="s">
         <v>30</v>
@@ -1901,21 +1904,21 @@
         <v>14</v>
       </c>
       <c r="G38" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H38" t="n">
         <v>4.859</v>
       </c>
       <c r="I38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C39" t="s">
         <v>11</v>
@@ -1930,21 +1933,21 @@
         <v>14</v>
       </c>
       <c r="G39" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H39" t="n">
         <v>1.077</v>
       </c>
       <c r="I39" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C40" t="s">
         <v>30</v>
@@ -1965,15 +1968,15 @@
         <v>8.822</v>
       </c>
       <c r="I40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
         <v>30</v>
@@ -1999,10 +2002,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
@@ -2016,8 +2019,8 @@
       <c r="F42" t="s">
         <v>20</v>
       </c>
-      <c r="G42" t="e">
-        <v>#N/A</v>
+      <c r="G42" t="s">
+        <v>21</v>
       </c>
       <c r="H42" t="e">
         <v>#N/A</v>
@@ -2028,10 +2031,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
@@ -2057,10 +2060,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
@@ -2086,10 +2089,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C45" t="s">
         <v>25</v>
@@ -2115,10 +2118,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
@@ -2139,15 +2142,15 @@
         <v>0.662</v>
       </c>
       <c r="I46" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C47" t="s">
         <v>11</v>
@@ -2168,15 +2171,15 @@
         <v>0.911</v>
       </c>
       <c r="I47" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B48" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
@@ -2197,15 +2200,15 @@
         <v>0.768</v>
       </c>
       <c r="I48" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C49" t="s">
         <v>30</v>
@@ -2220,21 +2223,21 @@
         <v>14</v>
       </c>
       <c r="G49" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H49" t="n">
         <v>1.494</v>
       </c>
       <c r="I49" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C50" t="s">
         <v>30</v>
@@ -2260,10 +2263,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B51" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
         <v>30</v>
@@ -2278,7 +2281,7 @@
         <v>20</v>
       </c>
       <c r="G51" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H51" t="n">
         <v>1.728</v>
@@ -2289,10 +2292,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B52" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
         <v>30</v>
@@ -2313,15 +2316,15 @@
         <v>0.954</v>
       </c>
       <c r="I52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B53" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C53" t="s">
         <v>30</v>
@@ -2342,15 +2345,15 @@
         <v>0.453</v>
       </c>
       <c r="I53" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C54" t="s">
         <v>11</v>
@@ -2365,7 +2368,7 @@
         <v>20</v>
       </c>
       <c r="G54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H54" t="e">
         <v>#N/A</v>
@@ -2376,10 +2379,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C55" t="s">
         <v>11</v>
@@ -2400,15 +2403,15 @@
         <v>0.409</v>
       </c>
       <c r="I55" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C56" t="s">
         <v>30</v>
@@ -2434,10 +2437,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B57" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C57" t="s">
         <v>11</v>
@@ -2452,24 +2455,24 @@
         <v>14</v>
       </c>
       <c r="G57" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H57" t="n">
         <v>1.733</v>
       </c>
       <c r="I57" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B58" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C58" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D58" t="s">
         <v>13</v>
@@ -2492,10 +2495,10 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B59" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C59" t="s">
         <v>11</v>
@@ -2516,15 +2519,15 @@
         <v>10.845</v>
       </c>
       <c r="I59" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B60" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C60" t="s">
         <v>11</v>
@@ -2545,15 +2548,15 @@
         <v>0.953</v>
       </c>
       <c r="I60" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B61" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C61" t="s">
         <v>30</v>
@@ -2574,15 +2577,15 @@
         <v>0.408</v>
       </c>
       <c r="I61" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B62" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C62" t="s">
         <v>11</v>
@@ -2603,15 +2606,15 @@
         <v>1.025</v>
       </c>
       <c r="I62" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B63" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C63" t="s">
         <v>11</v>
@@ -2632,7 +2635,7 @@
         <v>0.391</v>
       </c>
       <c r="I63" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add H3K27me3 result code to S1
Note, still two duplicates which need re-inspection of TMA
</commit_message>
<xml_diff>
--- a/analyses/11-tables/output/Table-S1.xlsx
+++ b/analyses/11-tables/output/Table-S1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t xml:space="preserve">Patient ID</t>
   </si>
@@ -32,6 +32,9 @@
     <t xml:space="preserve">ATRX IHC</t>
   </si>
   <si>
+    <t xml:space="preserve">H3K27me3 IHC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somatic ATRX</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
     <t xml:space="preserve">LOST</t>
   </si>
   <si>
+    <t xml:space="preserve">RETAINED</t>
+  </si>
+  <si>
     <t xml:space="preserve">p.R418*</t>
   </si>
   <si>
@@ -72,9 +78,6 @@
   </si>
   <si>
     <t xml:space="preserve">Not done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAINED</t>
   </si>
   <si>
     <t xml:space="preserve">Not mutated</t>
@@ -839,1582 +842,1747 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I6" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I8" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" t="e">
-        <v>#N/A</v>
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
       </c>
       <c r="H9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I9" t="s">
-        <v>16</v>
+      <c r="I9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I10" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
         <v>21</v>
       </c>
-      <c r="H11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I11" t="s">
-        <v>16</v>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I12" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I13" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" t="e">
-        <v>#N/A</v>
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
       </c>
       <c r="H14" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I14" t="s">
-        <v>16</v>
+      <c r="I14" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G15" t="s">
         <v>21</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" t="n">
         <v>0.55</v>
       </c>
-      <c r="I15" t="s">
-        <v>50</v>
+      <c r="J15" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G16" t="s">
         <v>21</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.989</v>
       </c>
-      <c r="I16" t="s">
-        <v>50</v>
+      <c r="J16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
         <v>54</v>
       </c>
-      <c r="B17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" t="n">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" t="n">
         <v>1.198</v>
       </c>
-      <c r="I17" t="s">
-        <v>50</v>
+      <c r="J17" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" t="e">
-        <v>#N/A</v>
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
       </c>
       <c r="H18" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I18" t="s">
-        <v>16</v>
+      <c r="I18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J18" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
         <v>21</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" t="n">
         <v>0.929</v>
       </c>
-      <c r="I19" t="s">
-        <v>50</v>
+      <c r="J19" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
         <v>62</v>
       </c>
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" t="s">
-        <v>61</v>
-      </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" t="e">
-        <v>#N/A</v>
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
       </c>
       <c r="H20" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I20" t="s">
-        <v>16</v>
+      <c r="I20" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J20" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>66</v>
-      </c>
-      <c r="H21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I21" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J21" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G22" t="s">
         <v>21</v>
       </c>
-      <c r="H22" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I22" t="s">
-        <v>16</v>
+      <c r="H22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" t="n">
+        <v>16</v>
+      </c>
+      <c r="H23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" t="n">
         <v>0.896</v>
       </c>
-      <c r="I23" t="s">
-        <v>50</v>
+      <c r="J23" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" t="n">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" t="n">
         <v>0.578</v>
       </c>
-      <c r="I24" t="s">
-        <v>50</v>
+      <c r="J24" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G25" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" t="n">
+        <v>16</v>
+      </c>
+      <c r="H25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" t="n">
         <v>0.765</v>
       </c>
-      <c r="I25" t="s">
-        <v>16</v>
+      <c r="J25" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
-      </c>
-      <c r="H26" t="n">
+        <v>16</v>
+      </c>
+      <c r="H26" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" t="n">
         <v>1.905</v>
       </c>
-      <c r="I26" t="s">
-        <v>50</v>
+      <c r="J26" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G27" t="s">
         <v>21</v>
       </c>
-      <c r="H27" t="n">
+      <c r="H27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" t="n">
         <v>0.785</v>
       </c>
-      <c r="I27" t="s">
-        <v>50</v>
+      <c r="J27" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G28" t="s">
-        <v>21</v>
-      </c>
-      <c r="H28" t="n">
+        <v>16</v>
+      </c>
+      <c r="H28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" t="n">
         <v>3.437</v>
       </c>
-      <c r="I28" t="s">
-        <v>50</v>
+      <c r="J28" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I29" t="s">
-        <v>16</v>
+        <v>16</v>
+      </c>
+      <c r="H29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J29" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G30" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" t="n">
+        <v>15</v>
+      </c>
+      <c r="H30" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" t="n">
         <v>0.724</v>
       </c>
-      <c r="I30" t="s">
-        <v>50</v>
+      <c r="J30" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" t="e">
-        <v>#N/A</v>
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>16</v>
       </c>
       <c r="H31" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I31" t="s">
-        <v>16</v>
+      <c r="I31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J31" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F32" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G32" t="s">
         <v>21</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" t="n">
         <v>0.883</v>
       </c>
-      <c r="I32" t="s">
-        <v>50</v>
+      <c r="J32" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G33" t="s">
-        <v>91</v>
-      </c>
-      <c r="H33" t="n">
+        <v>21</v>
+      </c>
+      <c r="H33" t="s">
+        <v>92</v>
+      </c>
+      <c r="I33" t="n">
         <v>2.78</v>
       </c>
-      <c r="I33" t="s">
-        <v>50</v>
+      <c r="J33" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G34" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" t="n">
+        <v>16</v>
+      </c>
+      <c r="H34" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" t="n">
         <v>0.665</v>
       </c>
-      <c r="I34" t="s">
-        <v>50</v>
+      <c r="J34" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G35" t="s">
-        <v>21</v>
-      </c>
-      <c r="H35" t="n">
+        <v>15</v>
+      </c>
+      <c r="H35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" t="n">
         <v>1.155</v>
       </c>
-      <c r="I35" t="s">
-        <v>50</v>
+      <c r="J35" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F36" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" t="e">
-        <v>#N/A</v>
+        <v>15</v>
+      </c>
+      <c r="G36" t="s">
+        <v>15</v>
       </c>
       <c r="H36" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I36" t="s">
-        <v>16</v>
+      <c r="I36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J36" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F37" t="s">
-        <v>20</v>
-      </c>
-      <c r="G37" t="e">
-        <v>#N/A</v>
+        <v>16</v>
+      </c>
+      <c r="G37" t="s">
+        <v>16</v>
       </c>
       <c r="H37" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I37" t="s">
-        <v>16</v>
+      <c r="I37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J37" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>102</v>
-      </c>
-      <c r="H38" t="n">
+        <v>16</v>
+      </c>
+      <c r="H38" t="s">
+        <v>103</v>
+      </c>
+      <c r="I38" t="n">
         <v>4.859</v>
       </c>
-      <c r="I38" t="s">
-        <v>50</v>
+      <c r="J38" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G39" t="s">
-        <v>105</v>
-      </c>
-      <c r="H39" t="n">
+        <v>15</v>
+      </c>
+      <c r="H39" t="s">
+        <v>106</v>
+      </c>
+      <c r="I39" t="n">
         <v>1.077</v>
       </c>
-      <c r="I39" t="s">
-        <v>50</v>
+      <c r="J39" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F40" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G40" t="s">
-        <v>21</v>
-      </c>
-      <c r="H40" t="n">
+        <v>16</v>
+      </c>
+      <c r="H40" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" t="n">
         <v>8.822</v>
       </c>
-      <c r="I40" t="s">
-        <v>50</v>
+      <c r="J40" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F41" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G41" t="s">
         <v>21</v>
       </c>
-      <c r="H41" t="n">
+      <c r="H41" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41" t="n">
         <v>4.079</v>
       </c>
-      <c r="I41" t="s">
-        <v>16</v>
+      <c r="J41" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F42" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G42" t="s">
         <v>21</v>
       </c>
-      <c r="H42" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I42" t="s">
-        <v>16</v>
+      <c r="H42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J42" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E43" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" t="e">
-        <v>#N/A</v>
+        <v>15</v>
+      </c>
+      <c r="G43" t="s">
+        <v>16</v>
       </c>
       <c r="H43" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I43" t="s">
-        <v>16</v>
+      <c r="I43" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J43" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F44" t="s">
-        <v>20</v>
-      </c>
-      <c r="G44" t="e">
-        <v>#N/A</v>
+        <v>16</v>
+      </c>
+      <c r="G44" t="s">
+        <v>15</v>
       </c>
       <c r="H44" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I44" t="s">
-        <v>16</v>
+      <c r="I44" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J44" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F45" t="s">
-        <v>19</v>
-      </c>
-      <c r="G45" t="e">
-        <v>#N/A</v>
+        <v>21</v>
+      </c>
+      <c r="G45" t="s">
+        <v>16</v>
       </c>
       <c r="H45" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I45" t="s">
-        <v>16</v>
+      <c r="I45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J45" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F46" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G46" t="s">
-        <v>21</v>
-      </c>
-      <c r="H46" t="n">
+        <v>15</v>
+      </c>
+      <c r="H46" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" t="n">
         <v>0.662</v>
       </c>
-      <c r="I46" t="s">
-        <v>50</v>
+      <c r="J46" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F47" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G47" t="s">
         <v>21</v>
       </c>
-      <c r="H47" t="n">
+      <c r="H47" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" t="n">
         <v>0.911</v>
       </c>
-      <c r="I47" t="s">
-        <v>50</v>
+      <c r="J47" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B48" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F48" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G48" t="s">
-        <v>21</v>
-      </c>
-      <c r="H48" t="n">
+        <v>16</v>
+      </c>
+      <c r="H48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" t="n">
         <v>0.768</v>
       </c>
-      <c r="I48" t="s">
-        <v>50</v>
+      <c r="J48" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C49" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F49" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G49" t="s">
-        <v>124</v>
-      </c>
-      <c r="H49" t="n">
+        <v>16</v>
+      </c>
+      <c r="H49" t="s">
+        <v>125</v>
+      </c>
+      <c r="I49" t="n">
         <v>1.494</v>
       </c>
-      <c r="I49" t="s">
-        <v>50</v>
+      <c r="J49" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C50" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D50" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E50" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F50" t="s">
-        <v>14</v>
-      </c>
-      <c r="G50" t="e">
-        <v>#N/A</v>
+        <v>15</v>
+      </c>
+      <c r="G50" t="s">
+        <v>16</v>
       </c>
       <c r="H50" t="e">
         <v>#N/A</v>
       </c>
-      <c r="I50" t="s">
-        <v>16</v>
+      <c r="I50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J50" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B51" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C51" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F51" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G51" t="s">
-        <v>129</v>
-      </c>
-      <c r="H51" t="n">
+        <v>15</v>
+      </c>
+      <c r="H51" t="s">
+        <v>130</v>
+      </c>
+      <c r="I51" t="n">
         <v>1.728</v>
       </c>
-      <c r="I51" t="s">
-        <v>16</v>
+      <c r="J51" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B52" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D52" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E52" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F52" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G52" t="s">
-        <v>21</v>
-      </c>
-      <c r="H52" t="n">
+        <v>16</v>
+      </c>
+      <c r="H52" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" t="n">
         <v>0.954</v>
       </c>
-      <c r="I52" t="s">
-        <v>50</v>
+      <c r="J52" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C53" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E53" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F53" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G53" t="s">
-        <v>21</v>
-      </c>
-      <c r="H53" t="n">
+        <v>16</v>
+      </c>
+      <c r="H53" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" t="n">
         <v>0.453</v>
       </c>
-      <c r="I53" t="s">
-        <v>50</v>
+      <c r="J53" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D54" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E54" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F54" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G54" t="s">
-        <v>136</v>
-      </c>
-      <c r="H54" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I54" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H54" t="s">
+        <v>137</v>
+      </c>
+      <c r="I54" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J54" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" t="s">
         <v>137</v>
       </c>
-      <c r="B55" t="s">
-        <v>138</v>
-      </c>
-      <c r="C55" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" t="s">
-        <v>12</v>
-      </c>
-      <c r="F55" t="s">
-        <v>20</v>
-      </c>
-      <c r="G55" t="s">
-        <v>21</v>
-      </c>
-      <c r="H55" t="n">
-        <v>0.409</v>
-      </c>
-      <c r="I55" t="s">
-        <v>50</v>
+      <c r="I55" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J55" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" t="s">
         <v>139</v>
       </c>
-      <c r="B56" t="s">
-        <v>140</v>
-      </c>
       <c r="C56" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -2423,27 +2591,30 @@
         <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G56" t="s">
-        <v>21</v>
-      </c>
-      <c r="H56" t="n">
-        <v>4.471</v>
-      </c>
-      <c r="I56" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H56" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.409</v>
+      </c>
+      <c r="J56" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B57" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D57" t="s">
         <v>13</v>
@@ -2452,190 +2623,275 @@
         <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G57" t="s">
-        <v>143</v>
-      </c>
-      <c r="H57" t="n">
-        <v>1.733</v>
-      </c>
-      <c r="I57" t="s">
-        <v>50</v>
+        <v>16</v>
+      </c>
+      <c r="H57" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.409</v>
+      </c>
+      <c r="J57" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B58" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C58" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="D58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F58" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G58" t="s">
-        <v>21</v>
-      </c>
-      <c r="H58" t="n">
-        <v>5.205</v>
-      </c>
-      <c r="I58" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="H58" t="s">
+        <v>22</v>
+      </c>
+      <c r="I58" t="n">
+        <v>4.471</v>
+      </c>
+      <c r="J58" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B59" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F59" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G59" t="s">
-        <v>21</v>
-      </c>
-      <c r="H59" t="n">
-        <v>10.845</v>
-      </c>
-      <c r="I59" t="s">
-        <v>50</v>
+        <v>15</v>
+      </c>
+      <c r="H59" t="s">
+        <v>144</v>
+      </c>
+      <c r="I59" t="n">
+        <v>1.733</v>
+      </c>
+      <c r="J59" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B60" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E60" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F60" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G60" t="s">
-        <v>21</v>
-      </c>
-      <c r="H60" t="n">
-        <v>0.953</v>
-      </c>
-      <c r="I60" t="s">
-        <v>50</v>
+        <v>16</v>
+      </c>
+      <c r="H60" t="s">
+        <v>22</v>
+      </c>
+      <c r="I60" t="n">
+        <v>5.205</v>
+      </c>
+      <c r="J60" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B61" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C61" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E61" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F61" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G61" t="s">
-        <v>21</v>
-      </c>
-      <c r="H61" t="n">
-        <v>0.408</v>
-      </c>
-      <c r="I61" t="s">
-        <v>50</v>
+        <v>16</v>
+      </c>
+      <c r="H61" t="s">
+        <v>22</v>
+      </c>
+      <c r="I61" t="n">
+        <v>10.845</v>
+      </c>
+      <c r="J61" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B62" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E62" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F62" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G62" t="s">
         <v>21</v>
       </c>
-      <c r="H62" t="n">
-        <v>1.025</v>
-      </c>
-      <c r="I62" t="s">
-        <v>50</v>
+      <c r="H62" t="s">
+        <v>22</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.953</v>
+      </c>
+      <c r="J62" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
+        <v>151</v>
+      </c>
+      <c r="B63" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" t="s">
+        <v>15</v>
+      </c>
+      <c r="H63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.408</v>
+      </c>
+      <c r="J63" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>153</v>
+      </c>
+      <c r="B64" t="s">
         <v>154</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" t="s">
+        <v>15</v>
+      </c>
+      <c r="H64" t="s">
+        <v>22</v>
+      </c>
+      <c r="I64" t="n">
+        <v>1.025</v>
+      </c>
+      <c r="J64" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
         <v>155</v>
       </c>
-      <c r="C63" t="s">
-        <v>11</v>
-      </c>
-      <c r="D63" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" t="s">
-        <v>12</v>
-      </c>
-      <c r="F63" t="s">
-        <v>20</v>
-      </c>
-      <c r="G63" t="s">
-        <v>21</v>
-      </c>
-      <c r="H63" t="n">
+      <c r="B65" t="s">
+        <v>156</v>
+      </c>
+      <c r="C65" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" t="s">
+        <v>15</v>
+      </c>
+      <c r="H65" t="s">
+        <v>22</v>
+      </c>
+      <c r="I65" t="n">
         <v>0.391</v>
       </c>
-      <c r="I63" t="s">
-        <v>50</v>
+      <c r="J65" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add tma + mut file, update S1
</commit_message>
<xml_diff>
--- a/analyses/11-tables/output/Table-S1.xlsx
+++ b/analyses/11-tables/output/Table-S1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
   <si>
     <t xml:space="preserve">Patient ID</t>
   </si>
@@ -32,12 +32,18 @@
     <t xml:space="preserve">ATRX IHC</t>
   </si>
   <si>
-    <t xml:space="preserve">H3K27me3 IHC</t>
-  </si>
-  <si>
     <t xml:space="preserve">Somatic ATRX</t>
   </si>
   <si>
+    <t xml:space="preserve">H3K28me3 IHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3K28M IHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somatic H3</t>
+  </si>
+  <si>
     <t xml:space="preserve">T/N TelHunt ratio</t>
   </si>
   <si>
@@ -62,10 +68,13 @@
     <t xml:space="preserve">LOST</t>
   </si>
   <si>
+    <t xml:space="preserve">p.R418*</t>
+  </si>
+  <si>
     <t xml:space="preserve">RETAINED</t>
   </si>
   <si>
-    <t xml:space="preserve">p.R418*</t>
+    <t xml:space="preserve">H3-wildtype</t>
   </si>
   <si>
     <t xml:space="preserve">Validation</t>
@@ -83,6 +92,12 @@
     <t xml:space="preserve">Not mutated</t>
   </si>
   <si>
+    <t xml:space="preserve">K28-altered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3F3A p.K28M</t>
+  </si>
+  <si>
     <t xml:space="preserve">C1061121</t>
   </si>
   <si>
@@ -132,6 +147,9 @@
   </si>
   <si>
     <t xml:space="preserve">p.S930Ffs*7, p.E929Qfs*8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3F3A p.G35R</t>
   </si>
   <si>
     <t xml:space="preserve">C1190886</t>
@@ -845,2053 +863,2367 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="e">
-        <v>#N/A</v>
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="K2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L4" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="e">
-        <v>#N/A</v>
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="K5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="s">
         <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L7" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" t="e">
-        <v>#N/A</v>
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="K8" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J9" t="s">
-        <v>18</v>
+      <c r="J9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" t="e">
-        <v>#N/A</v>
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>18</v>
+        <v>45</v>
+      </c>
+      <c r="K10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L11" t="s">
         <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" t="e">
-        <v>#N/A</v>
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>20</v>
       </c>
       <c r="J12" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="K12" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" t="e">
-        <v>#N/A</v>
+        <v>19</v>
+      </c>
+      <c r="I13" t="s">
+        <v>20</v>
       </c>
       <c r="J13" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="K13" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J14" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="G14" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K14" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" t="n">
+        <v>19</v>
+      </c>
+      <c r="I15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" t="n">
         <v>0.55</v>
       </c>
-      <c r="J15" t="s">
-        <v>51</v>
+      <c r="L15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H16" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" t="n">
+        <v>19</v>
+      </c>
+      <c r="I16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" t="n">
         <v>0.989</v>
       </c>
-      <c r="J16" t="s">
-        <v>51</v>
+      <c r="L16" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="H17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1.198</v>
+      </c>
+      <c r="L17" t="s">
         <v>57</v>
-      </c>
-      <c r="I17" t="n">
-        <v>1.198</v>
-      </c>
-      <c r="J17" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L18" t="s">
         <v>21</v>
-      </c>
-      <c r="H18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J18" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" t="n">
+        <v>25</v>
+      </c>
+      <c r="H19" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I19" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J19" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" t="n">
         <v>0.929</v>
       </c>
-      <c r="J19" t="s">
-        <v>51</v>
+      <c r="L19" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I20" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J20" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="G20" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K20" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L20" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="H21" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21" t="e">
-        <v>#N/A</v>
+        <v>19</v>
+      </c>
+      <c r="I21" t="s">
+        <v>20</v>
       </c>
       <c r="J21" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="K21" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L21" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L22" t="s">
         <v>21</v>
-      </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J22" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H23" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" t="n">
+        <v>19</v>
+      </c>
+      <c r="I23" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J23" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" t="n">
         <v>0.896</v>
       </c>
-      <c r="J23" t="s">
-        <v>51</v>
+      <c r="L23" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G24" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H24" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" t="n">
+        <v>19</v>
+      </c>
+      <c r="I24" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" t="n">
         <v>0.578</v>
       </c>
-      <c r="J24" t="s">
-        <v>51</v>
+      <c r="L24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G25" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" t="n">
+        <v>19</v>
+      </c>
+      <c r="I25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" t="n">
         <v>0.765</v>
       </c>
-      <c r="J25" t="s">
-        <v>18</v>
+      <c r="L25" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G26" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="H26" t="s">
-        <v>77</v>
-      </c>
-      <c r="I26" t="n">
+        <v>19</v>
+      </c>
+      <c r="I26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" t="n">
         <v>1.905</v>
       </c>
-      <c r="J26" t="s">
-        <v>51</v>
+      <c r="L26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G27" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" t="n">
+        <v>19</v>
+      </c>
+      <c r="I27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" t="n">
         <v>0.785</v>
       </c>
-      <c r="J27" t="s">
-        <v>51</v>
+      <c r="L27" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G28" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" t="n">
+        <v>19</v>
+      </c>
+      <c r="I28" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" t="n">
         <v>3.437</v>
       </c>
-      <c r="J28" t="s">
-        <v>51</v>
+      <c r="L28" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G29" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H29" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" t="e">
-        <v>#N/A</v>
+        <v>19</v>
+      </c>
+      <c r="I29" t="s">
+        <v>20</v>
       </c>
       <c r="J29" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="K29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L29" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I30" t="n">
+        <v>17</v>
+      </c>
+      <c r="I30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" t="s">
+        <v>27</v>
+      </c>
+      <c r="K30" t="n">
         <v>0.724</v>
       </c>
-      <c r="J30" t="s">
-        <v>51</v>
+      <c r="L30" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K31" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L31" t="s">
         <v>21</v>
-      </c>
-      <c r="E31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J31" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F32" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G32" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H32" t="s">
-        <v>22</v>
-      </c>
-      <c r="I32" t="n">
+        <v>19</v>
+      </c>
+      <c r="I32" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" t="n">
         <v>0.883</v>
       </c>
-      <c r="J32" t="s">
-        <v>51</v>
+      <c r="L32" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F33" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G33" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="H33" t="s">
-        <v>92</v>
-      </c>
-      <c r="I33" t="n">
+        <v>19</v>
+      </c>
+      <c r="I33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" t="s">
+        <v>45</v>
+      </c>
+      <c r="K33" t="n">
         <v>2.78</v>
       </c>
-      <c r="J33" t="s">
-        <v>51</v>
+      <c r="L33" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F34" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G34" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H34" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34" t="n">
+        <v>19</v>
+      </c>
+      <c r="I34" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" t="s">
+        <v>20</v>
+      </c>
+      <c r="K34" t="n">
         <v>0.665</v>
       </c>
-      <c r="J34" t="s">
-        <v>51</v>
+      <c r="L34" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F35" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G35" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35" t="n">
+        <v>17</v>
+      </c>
+      <c r="I35" t="s">
+        <v>26</v>
+      </c>
+      <c r="J35" t="s">
+        <v>27</v>
+      </c>
+      <c r="K35" t="n">
         <v>1.155</v>
       </c>
-      <c r="J35" t="s">
-        <v>51</v>
+      <c r="L35" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F36" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" t="e">
-        <v>#N/A</v>
+        <v>17</v>
+      </c>
+      <c r="G36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H36" t="s">
+        <v>17</v>
       </c>
       <c r="I36" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J36" t="s">
-        <v>18</v>
+      <c r="J36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L36" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D37" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H37" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L37" t="s">
         <v>21</v>
-      </c>
-      <c r="E37" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I37" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J37" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F38" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G38" t="s">
-        <v>16</v>
+        <v>109</v>
       </c>
       <c r="H38" t="s">
-        <v>103</v>
-      </c>
-      <c r="I38" t="n">
+        <v>19</v>
+      </c>
+      <c r="I38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" t="n">
         <v>4.859</v>
       </c>
-      <c r="J38" t="s">
-        <v>51</v>
+      <c r="L38" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F39" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" t="s">
-        <v>106</v>
-      </c>
-      <c r="I39" t="n">
+        <v>112</v>
+      </c>
+      <c r="H39" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K39" t="n">
         <v>1.077</v>
       </c>
-      <c r="J39" t="s">
-        <v>51</v>
+      <c r="L39" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F40" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G40" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H40" t="s">
-        <v>22</v>
-      </c>
-      <c r="I40" t="n">
+        <v>19</v>
+      </c>
+      <c r="I40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" t="n">
         <v>8.822</v>
       </c>
-      <c r="J40" t="s">
-        <v>51</v>
+      <c r="L40" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F41" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" t="s">
+        <v>19</v>
+      </c>
+      <c r="I41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" t="s">
+        <v>20</v>
+      </c>
+      <c r="K41" t="n">
+        <v>4.079</v>
+      </c>
+      <c r="L41" t="s">
         <v>21</v>
-      </c>
-      <c r="G41" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" t="s">
-        <v>22</v>
-      </c>
-      <c r="I41" t="n">
-        <v>4.079</v>
-      </c>
-      <c r="J41" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" t="s">
+        <v>20</v>
+      </c>
+      <c r="J42" t="s">
+        <v>20</v>
+      </c>
+      <c r="K42" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L42" t="s">
         <v>21</v>
-      </c>
-      <c r="E42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" t="s">
-        <v>21</v>
-      </c>
-      <c r="H42" t="s">
-        <v>22</v>
-      </c>
-      <c r="I42" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J42" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E43" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H43" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" t="s">
+        <v>20</v>
+      </c>
+      <c r="J43" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K43" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L43" t="s">
         <v>21</v>
-      </c>
-      <c r="F43" t="s">
-        <v>15</v>
-      </c>
-      <c r="G43" t="s">
-        <v>16</v>
-      </c>
-      <c r="H43" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I43" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J43" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F44" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H44" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I44" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J44" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="G44" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H44" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" t="s">
+        <v>26</v>
+      </c>
+      <c r="J44" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K44" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L44" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C45" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E45" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F45" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H45" t="s">
+        <v>19</v>
+      </c>
+      <c r="I45" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L45" t="s">
         <v>21</v>
-      </c>
-      <c r="G45" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I45" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J45" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B46" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F46" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G46" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H46" t="s">
-        <v>22</v>
-      </c>
-      <c r="I46" t="n">
+        <v>17</v>
+      </c>
+      <c r="I46" t="s">
+        <v>26</v>
+      </c>
+      <c r="J46" t="s">
+        <v>27</v>
+      </c>
+      <c r="K46" t="n">
         <v>0.662</v>
       </c>
-      <c r="J46" t="s">
-        <v>51</v>
+      <c r="L46" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F47" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G47" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H47" t="s">
-        <v>22</v>
-      </c>
-      <c r="I47" t="n">
+        <v>19</v>
+      </c>
+      <c r="I47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" t="s">
+        <v>20</v>
+      </c>
+      <c r="K47" t="n">
         <v>0.911</v>
       </c>
-      <c r="J47" t="s">
-        <v>51</v>
+      <c r="L47" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F48" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G48" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H48" t="s">
-        <v>22</v>
-      </c>
-      <c r="I48" t="n">
+        <v>19</v>
+      </c>
+      <c r="I48" t="s">
+        <v>20</v>
+      </c>
+      <c r="J48" t="s">
+        <v>20</v>
+      </c>
+      <c r="K48" t="n">
         <v>0.768</v>
       </c>
-      <c r="J48" t="s">
-        <v>51</v>
+      <c r="L48" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D49" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E49" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F49" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G49" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
       <c r="H49" t="s">
-        <v>125</v>
-      </c>
-      <c r="I49" t="n">
+        <v>19</v>
+      </c>
+      <c r="I49" t="s">
+        <v>20</v>
+      </c>
+      <c r="J49" t="s">
+        <v>20</v>
+      </c>
+      <c r="K49" t="n">
         <v>1.494</v>
       </c>
-      <c r="J49" t="s">
-        <v>51</v>
+      <c r="L49" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B50" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C50" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F50" t="s">
-        <v>15</v>
-      </c>
-      <c r="G50" t="s">
-        <v>16</v>
-      </c>
-      <c r="H50" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I50" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J50" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="G50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H50" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L50" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C51" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E51" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F51" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G51" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="H51" t="s">
-        <v>130</v>
-      </c>
-      <c r="I51" t="n">
+        <v>17</v>
+      </c>
+      <c r="I51" t="s">
+        <v>26</v>
+      </c>
+      <c r="J51" t="s">
+        <v>27</v>
+      </c>
+      <c r="K51" t="n">
         <v>1.728</v>
       </c>
-      <c r="J51" t="s">
-        <v>18</v>
+      <c r="L51" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C52" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E52" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F52" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G52" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H52" t="s">
-        <v>22</v>
-      </c>
-      <c r="I52" t="n">
+        <v>19</v>
+      </c>
+      <c r="I52" t="s">
+        <v>20</v>
+      </c>
+      <c r="J52" t="s">
+        <v>20</v>
+      </c>
+      <c r="K52" t="n">
         <v>0.954</v>
       </c>
-      <c r="J52" t="s">
-        <v>51</v>
+      <c r="L52" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C53" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D53" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E53" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F53" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G53" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H53" t="s">
-        <v>22</v>
-      </c>
-      <c r="I53" t="n">
+        <v>19</v>
+      </c>
+      <c r="I53" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53" t="s">
+        <v>20</v>
+      </c>
+      <c r="K53" t="n">
         <v>0.453</v>
       </c>
-      <c r="J53" t="s">
-        <v>51</v>
+      <c r="L53" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B54" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D54" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" t="s">
+        <v>143</v>
+      </c>
+      <c r="H54" t="s">
+        <v>17</v>
+      </c>
+      <c r="I54" t="s">
+        <v>26</v>
+      </c>
+      <c r="J54" t="s">
+        <v>20</v>
+      </c>
+      <c r="K54" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L54" t="s">
         <v>21</v>
-      </c>
-      <c r="E54" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" t="s">
-        <v>16</v>
-      </c>
-      <c r="G54" t="s">
-        <v>15</v>
-      </c>
-      <c r="H54" t="s">
-        <v>137</v>
-      </c>
-      <c r="I54" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J54" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B55" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D55" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E55" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F55" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G55" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H55" t="s">
-        <v>137</v>
-      </c>
-      <c r="I55" t="e">
-        <v>#N/A</v>
+        <v>17</v>
+      </c>
+      <c r="I55" t="s">
+        <v>20</v>
       </c>
       <c r="J55" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.409</v>
+      </c>
+      <c r="L55" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="D56" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E56" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F56" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G56" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H56" t="s">
-        <v>22</v>
-      </c>
-      <c r="I56" t="n">
-        <v>0.409</v>
+        <v>17</v>
+      </c>
+      <c r="I56" t="s">
+        <v>26</v>
       </c>
       <c r="J56" t="s">
-        <v>51</v>
+        <v>20</v>
+      </c>
+      <c r="K56" t="n">
+        <v>4.471</v>
+      </c>
+      <c r="L56" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C57" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D57" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F57" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G57" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="H57" t="s">
-        <v>22</v>
-      </c>
-      <c r="I57" t="n">
-        <v>0.409</v>
+        <v>17</v>
+      </c>
+      <c r="I57" t="s">
+        <v>26</v>
       </c>
       <c r="J57" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="K57" t="n">
+        <v>1.733</v>
+      </c>
+      <c r="L57" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B58" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="C58" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="D58" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E58" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F58" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G58" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H58" t="s">
-        <v>22</v>
-      </c>
-      <c r="I58" t="n">
-        <v>4.471</v>
+        <v>19</v>
+      </c>
+      <c r="I58" t="s">
+        <v>20</v>
       </c>
       <c r="J58" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="K58" t="n">
+        <v>5.205</v>
+      </c>
+      <c r="L58" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="C59" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D59" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E59" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F59" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G59" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H59" t="s">
-        <v>144</v>
-      </c>
-      <c r="I59" t="n">
-        <v>1.733</v>
+        <v>19</v>
+      </c>
+      <c r="I59" t="s">
+        <v>20</v>
       </c>
       <c r="J59" t="s">
-        <v>51</v>
+        <v>20</v>
+      </c>
+      <c r="K59" t="n">
+        <v>10.845</v>
+      </c>
+      <c r="L59" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B60" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="C60" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E60" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F60" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G60" t="s">
-        <v>16</v>
-      </c>
-      <c r="H60" t="s">
-        <v>22</v>
-      </c>
-      <c r="I60" t="n">
-        <v>5.205</v>
+        <v>25</v>
+      </c>
+      <c r="H60" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I60" t="s">
+        <v>20</v>
       </c>
       <c r="J60" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.953</v>
+      </c>
+      <c r="L60" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="B61" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C61" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="D61" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E61" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F61" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G61" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H61" t="s">
-        <v>22</v>
-      </c>
-      <c r="I61" t="n">
-        <v>10.845</v>
+        <v>17</v>
+      </c>
+      <c r="I61" t="s">
+        <v>26</v>
       </c>
       <c r="J61" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.408</v>
+      </c>
+      <c r="L61" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B62" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C62" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E62" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F62" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G62" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H62" t="s">
-        <v>22</v>
-      </c>
-      <c r="I62" t="n">
-        <v>0.953</v>
+        <v>17</v>
+      </c>
+      <c r="I62" t="s">
+        <v>26</v>
       </c>
       <c r="J62" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="K62" t="n">
+        <v>1.025</v>
+      </c>
+      <c r="L62" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B63" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C63" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E63" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F63" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G63" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H63" t="s">
-        <v>22</v>
-      </c>
-      <c r="I63" t="n">
-        <v>0.408</v>
+        <v>17</v>
+      </c>
+      <c r="I63" t="s">
+        <v>26</v>
       </c>
       <c r="J63" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>153</v>
-      </c>
-      <c r="B64" t="s">
-        <v>154</v>
-      </c>
-      <c r="C64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D64" t="s">
-        <v>13</v>
-      </c>
-      <c r="E64" t="s">
-        <v>13</v>
-      </c>
-      <c r="F64" t="s">
-        <v>16</v>
-      </c>
-      <c r="G64" t="s">
-        <v>15</v>
-      </c>
-      <c r="H64" t="s">
-        <v>22</v>
-      </c>
-      <c r="I64" t="n">
-        <v>1.025</v>
-      </c>
-      <c r="J64" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>155</v>
-      </c>
-      <c r="B65" t="s">
-        <v>156</v>
-      </c>
-      <c r="C65" t="s">
-        <v>12</v>
-      </c>
-      <c r="D65" t="s">
-        <v>13</v>
-      </c>
-      <c r="E65" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" t="s">
-        <v>16</v>
-      </c>
-      <c r="G65" t="s">
-        <v>15</v>
-      </c>
-      <c r="H65" t="s">
-        <v>22</v>
-      </c>
-      <c r="I65" t="n">
+        <v>27</v>
+      </c>
+      <c r="K63" t="n">
         <v>0.391</v>
       </c>
-      <c r="J65" t="s">
-        <v>51</v>
+      <c r="L63" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add cns regions to table S1
</commit_message>
<xml_diff>
--- a/analyses/11-tables/output/Table-S1.xlsx
+++ b/analyses/11-tables/output/Table-S1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
   <si>
     <t xml:space="preserve">Patient ID</t>
   </si>
@@ -95,6 +95,9 @@
     <t xml:space="preserve">7316-4335</t>
   </si>
   <si>
+    <t xml:space="preserve">Midline</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not done</t>
   </si>
   <si>
@@ -152,6 +155,9 @@
     <t xml:space="preserve">7316-486</t>
   </si>
   <si>
+    <t xml:space="preserve">Spine</t>
+  </si>
+  <si>
     <t xml:space="preserve">C1174527</t>
   </si>
   <si>
@@ -216,9 +222,6 @@
   </si>
   <si>
     <t xml:space="preserve">7316-903</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Midline</t>
   </si>
   <si>
     <t xml:space="preserve">p.D1714V (VUS)</t>
@@ -945,11 +948,11 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="e">
-        <v>#N/A</v>
+      <c r="D3" t="s">
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -958,16 +961,16 @@
         <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L3" t="e">
         <v>#N/A</v>
@@ -978,19 +981,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -999,7 +1002,7 @@
         <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
         <v>21</v>
@@ -1019,17 +1022,17 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
         <v>21</v>
@@ -1060,19 +1063,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="e">
-        <v>#N/A</v>
+      <c r="D6" t="s">
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -1081,7 +1084,7 @@
         <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I6" t="s">
         <v>21</v>
@@ -1101,19 +1104,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -1122,7 +1125,7 @@
         <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I7" t="s">
         <v>21</v>
@@ -1142,16 +1145,16 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="e">
-        <v>#N/A</v>
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
@@ -1163,7 +1166,7 @@
         <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I8" t="s">
         <v>21</v>
@@ -1183,16 +1186,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="e">
-        <v>#N/A</v>
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
       </c>
       <c r="E9" t="s">
         <v>17</v>
@@ -1210,7 +1213,7 @@
         <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K9" t="e">
         <v>#N/A</v>
@@ -1224,16 +1227,16 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
@@ -1245,7 +1248,7 @@
         <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
         <v>21</v>
@@ -1254,7 +1257,7 @@
         <v>22</v>
       </c>
       <c r="K10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L10" t="e">
         <v>#N/A</v>
@@ -1265,19 +1268,19 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" t="e">
-        <v>#N/A</v>
+      <c r="D11" t="s">
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
         <v>18</v>
@@ -1286,7 +1289,7 @@
         <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I11" t="e">
         <v>#N/A</v>
@@ -1295,7 +1298,7 @@
         <v>#N/A</v>
       </c>
       <c r="K11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L11" t="e">
         <v>#N/A</v>
@@ -1306,16 +1309,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" t="e">
-        <v>#N/A</v>
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
@@ -1327,7 +1330,7 @@
         <v>21</v>
       </c>
       <c r="H12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I12" t="s">
         <v>21</v>
@@ -1347,16 +1350,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
@@ -1368,7 +1371,7 @@
         <v>21</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I13" t="s">
         <v>21</v>
@@ -1388,16 +1391,16 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
@@ -1429,16 +1432,16 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
         <v>17</v>
@@ -1450,7 +1453,7 @@
         <v>21</v>
       </c>
       <c r="H15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I15" t="s">
         <v>21</v>
@@ -1465,21 +1468,21 @@
         <v>0.55</v>
       </c>
       <c r="M15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
         <v>17</v>
@@ -1491,7 +1494,7 @@
         <v>21</v>
       </c>
       <c r="H16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I16" t="s">
         <v>21</v>
@@ -1506,62 +1509,62 @@
         <v>0.989</v>
       </c>
       <c r="M16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
         <v>66</v>
       </c>
-      <c r="B17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
         <v>17</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G17" t="s">
         <v>21</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I17" t="s">
         <v>19</v>
       </c>
       <c r="J17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L17" t="n">
         <v>1.198</v>
       </c>
       <c r="M17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
         <v>17</v>
@@ -1593,16 +1596,16 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
@@ -1614,7 +1617,7 @@
         <v>21</v>
       </c>
       <c r="H19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I19" t="e">
         <v>#N/A</v>
@@ -1629,21 +1632,21 @@
         <v>0.929</v>
       </c>
       <c r="M19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
         <v>76</v>
       </c>
-      <c r="B20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
@@ -1675,13 +1678,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21" t="e">
         <v>#N/A</v>
@@ -1696,7 +1699,7 @@
         <v>19</v>
       </c>
       <c r="H21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I21" t="s">
         <v>21</v>
@@ -1716,10 +1719,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
@@ -1728,7 +1731,7 @@
         <v>#N/A</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F22" t="s">
         <v>18</v>
@@ -1737,16 +1740,16 @@
         <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I22" t="s">
         <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L22" t="e">
         <v>#N/A</v>
@@ -1757,16 +1760,16 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
         <v>17</v>
@@ -1778,7 +1781,7 @@
         <v>21</v>
       </c>
       <c r="H23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I23" t="s">
         <v>21</v>
@@ -1793,21 +1796,21 @@
         <v>0.896</v>
       </c>
       <c r="M23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
         <v>17</v>
@@ -1819,7 +1822,7 @@
         <v>21</v>
       </c>
       <c r="H24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I24" t="s">
         <v>21</v>
@@ -1834,21 +1837,21 @@
         <v>0.578</v>
       </c>
       <c r="M24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
         <v>17</v>
@@ -1860,7 +1863,7 @@
         <v>21</v>
       </c>
       <c r="H25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I25" t="s">
         <v>21</v>
@@ -1880,16 +1883,16 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
         <v>18</v>
@@ -1901,7 +1904,7 @@
         <v>19</v>
       </c>
       <c r="H26" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I26" t="s">
         <v>21</v>
@@ -1916,21 +1919,21 @@
         <v>1.905</v>
       </c>
       <c r="M26" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
         <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
         <v>17</v>
@@ -1942,7 +1945,7 @@
         <v>21</v>
       </c>
       <c r="H27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I27" t="s">
         <v>21</v>
@@ -1957,21 +1960,21 @@
         <v>0.785</v>
       </c>
       <c r="M27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E28" t="s">
         <v>18</v>
@@ -1983,7 +1986,7 @@
         <v>21</v>
       </c>
       <c r="H28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I28" t="s">
         <v>21</v>
@@ -1998,21 +2001,21 @@
         <v>3.437</v>
       </c>
       <c r="M28" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E29" t="s">
         <v>18</v>
@@ -2024,7 +2027,7 @@
         <v>21</v>
       </c>
       <c r="H29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I29" t="s">
         <v>21</v>
@@ -2044,16 +2047,16 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E30" t="s">
         <v>17</v>
@@ -2065,39 +2068,39 @@
         <v>21</v>
       </c>
       <c r="H30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I30" t="s">
         <v>19</v>
       </c>
       <c r="J30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L30" t="n">
         <v>0.724</v>
       </c>
       <c r="M30" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" t="e">
-        <v>#N/A</v>
+        <v>36</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F31" t="s">
         <v>17</v>
@@ -2126,16 +2129,16 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
         <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
         <v>17</v>
@@ -2147,7 +2150,7 @@
         <v>21</v>
       </c>
       <c r="H32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I32" t="s">
         <v>21</v>
@@ -2162,21 +2165,21 @@
         <v>0.883</v>
       </c>
       <c r="M32" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
         <v>18</v>
@@ -2188,7 +2191,7 @@
         <v>19</v>
       </c>
       <c r="H33" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I33" t="s">
         <v>21</v>
@@ -2197,27 +2200,27 @@
         <v>22</v>
       </c>
       <c r="K33" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L33" t="n">
         <v>2.78</v>
       </c>
       <c r="M33" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
         <v>17</v>
@@ -2229,7 +2232,7 @@
         <v>21</v>
       </c>
       <c r="H34" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I34" t="s">
         <v>21</v>
@@ -2244,21 +2247,21 @@
         <v>0.665</v>
       </c>
       <c r="M34" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C35" t="s">
         <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E35" t="s">
         <v>17</v>
@@ -2270,36 +2273,36 @@
         <v>21</v>
       </c>
       <c r="H35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I35" t="s">
         <v>19</v>
       </c>
       <c r="J35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K35" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L35" t="n">
         <v>1.155</v>
       </c>
       <c r="M35" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E36" t="s">
         <v>18</v>
@@ -2331,19 +2334,19 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C37" t="s">
         <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F37" t="s">
         <v>17</v>
@@ -2372,16 +2375,16 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
         <v>18</v>
@@ -2393,7 +2396,7 @@
         <v>19</v>
       </c>
       <c r="H38" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I38" t="s">
         <v>21</v>
@@ -2408,21 +2411,21 @@
         <v>4.859</v>
       </c>
       <c r="M38" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C39" t="s">
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E39" t="s">
         <v>18</v>
@@ -2434,36 +2437,36 @@
         <v>19</v>
       </c>
       <c r="H39" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I39" t="s">
         <v>19</v>
       </c>
       <c r="J39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L39" t="n">
         <v>1.077</v>
       </c>
       <c r="M39" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B40" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E40" t="s">
         <v>18</v>
@@ -2475,7 +2478,7 @@
         <v>21</v>
       </c>
       <c r="H40" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I40" t="s">
         <v>21</v>
@@ -2490,21 +2493,21 @@
         <v>8.822</v>
       </c>
       <c r="M40" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E41" t="s">
         <v>18</v>
@@ -2513,10 +2516,10 @@
         <v>18</v>
       </c>
       <c r="G41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H41" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I41" t="s">
         <v>21</v>
@@ -2536,19 +2539,19 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" t="e">
-        <v>#N/A</v>
+        <v>36</v>
+      </c>
+      <c r="D42" t="s">
+        <v>27</v>
       </c>
       <c r="E42" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F42" t="s">
         <v>18</v>
@@ -2557,7 +2560,7 @@
         <v>21</v>
       </c>
       <c r="H42" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I42" t="s">
         <v>21</v>
@@ -2577,22 +2580,22 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B43" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C43" t="s">
         <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E43" t="s">
         <v>18</v>
       </c>
       <c r="F43" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G43" t="s">
         <v>19</v>
@@ -2618,16 +2621,16 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C44" t="s">
         <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E44" t="s">
         <v>18</v>
@@ -2645,7 +2648,7 @@
         <v>19</v>
       </c>
       <c r="J44" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K44" t="e">
         <v>#N/A</v>
@@ -2659,16 +2662,16 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
-      </c>
-      <c r="D45" t="e">
-        <v>#N/A</v>
+        <v>36</v>
+      </c>
+      <c r="D45" t="s">
+        <v>47</v>
       </c>
       <c r="E45" t="s">
         <v>17</v>
@@ -2677,7 +2680,7 @@
         <v>17</v>
       </c>
       <c r="G45" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H45" t="e">
         <v>#N/A</v>
@@ -2700,16 +2703,16 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B46" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C46" t="s">
         <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E46" t="s">
         <v>17</v>
@@ -2721,36 +2724,36 @@
         <v>21</v>
       </c>
       <c r="H46" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I46" t="s">
         <v>19</v>
       </c>
       <c r="J46" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K46" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L46" t="n">
         <v>0.662</v>
       </c>
       <c r="M46" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B47" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C47" t="s">
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E47" t="s">
         <v>17</v>
@@ -2762,7 +2765,7 @@
         <v>21</v>
       </c>
       <c r="H47" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I47" t="s">
         <v>21</v>
@@ -2777,21 +2780,21 @@
         <v>0.911</v>
       </c>
       <c r="M47" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E48" t="s">
         <v>17</v>
@@ -2803,7 +2806,7 @@
         <v>21</v>
       </c>
       <c r="H48" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I48" t="s">
         <v>21</v>
@@ -2818,21 +2821,21 @@
         <v>0.768</v>
       </c>
       <c r="M48" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B49" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C49" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E49" t="s">
         <v>17</v>
@@ -2844,7 +2847,7 @@
         <v>19</v>
       </c>
       <c r="H49" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I49" t="s">
         <v>21</v>
@@ -2859,21 +2862,21 @@
         <v>1.494</v>
       </c>
       <c r="M49" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B50" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C50" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D50" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E50" t="s">
         <v>17</v>
@@ -2905,16 +2908,16 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D51" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E51" t="s">
         <v>18</v>
@@ -2926,16 +2929,16 @@
         <v>21</v>
       </c>
       <c r="H51" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I51" t="s">
         <v>19</v>
       </c>
       <c r="J51" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K51" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L51" t="n">
         <v>1.728</v>
@@ -2946,28 +2949,28 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E52" t="s">
         <v>17</v>
       </c>
       <c r="F52" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G52" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H52" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I52" t="s">
         <v>21</v>
@@ -2982,21 +2985,21 @@
         <v>0.954</v>
       </c>
       <c r="M52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B53" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E53" t="s">
         <v>17</v>
@@ -3008,7 +3011,7 @@
         <v>21</v>
       </c>
       <c r="H53" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I53" t="s">
         <v>21</v>
@@ -3023,24 +3026,24 @@
         <v>0.453</v>
       </c>
       <c r="M53" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B54" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C54" t="s">
         <v>15</v>
       </c>
-      <c r="D54" t="e">
-        <v>#N/A</v>
+      <c r="D54" t="s">
+        <v>27</v>
       </c>
       <c r="E54" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F54" t="s">
         <v>17</v>
@@ -3049,7 +3052,7 @@
         <v>21</v>
       </c>
       <c r="H54" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I54" t="s">
         <v>19</v>
@@ -3069,16 +3072,16 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B55" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C55" t="s">
         <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E55" t="s">
         <v>17</v>
@@ -3090,7 +3093,7 @@
         <v>21</v>
       </c>
       <c r="H55" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I55" t="s">
         <v>19</v>
@@ -3105,21 +3108,21 @@
         <v>0.409</v>
       </c>
       <c r="M55" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B56" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C56" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D56" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E56" t="s">
         <v>18</v>
@@ -3131,16 +3134,16 @@
         <v>21</v>
       </c>
       <c r="H56" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I56" t="s">
         <v>19</v>
       </c>
       <c r="J56" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K56" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L56" t="n">
         <v>4.471</v>
@@ -3151,16 +3154,16 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B57" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E57" t="s">
         <v>18</v>
@@ -3172,36 +3175,36 @@
         <v>19</v>
       </c>
       <c r="H57" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I57" t="s">
         <v>19</v>
       </c>
       <c r="J57" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K57" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L57" t="n">
         <v>1.733</v>
       </c>
       <c r="M57" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B58" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D58" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E58" t="s">
         <v>18</v>
@@ -3213,7 +3216,7 @@
         <v>21</v>
       </c>
       <c r="H58" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I58" t="s">
         <v>21</v>
@@ -3233,16 +3236,16 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B59" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C59" t="s">
         <v>15</v>
       </c>
       <c r="D59" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E59" t="s">
         <v>18</v>
@@ -3254,7 +3257,7 @@
         <v>21</v>
       </c>
       <c r="H59" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I59" t="s">
         <v>21</v>
@@ -3269,21 +3272,21 @@
         <v>10.845</v>
       </c>
       <c r="M59" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B60" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C60" t="s">
         <v>15</v>
       </c>
       <c r="D60" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E60" t="s">
         <v>17</v>
@@ -3295,7 +3298,7 @@
         <v>21</v>
       </c>
       <c r="H60" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I60" t="e">
         <v>#N/A</v>
@@ -3310,21 +3313,21 @@
         <v>0.953</v>
       </c>
       <c r="M60" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B61" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C61" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D61" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E61" t="s">
         <v>17</v>
@@ -3336,36 +3339,36 @@
         <v>21</v>
       </c>
       <c r="H61" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I61" t="s">
         <v>19</v>
       </c>
       <c r="J61" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K61" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L61" t="n">
         <v>0.408</v>
       </c>
       <c r="M61" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B62" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C62" t="s">
         <v>15</v>
       </c>
       <c r="D62" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E62" t="s">
         <v>17</v>
@@ -3377,36 +3380,36 @@
         <v>21</v>
       </c>
       <c r="H62" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I62" t="s">
         <v>19</v>
       </c>
       <c r="J62" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K62" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L62" t="n">
         <v>1.025</v>
       </c>
       <c r="M62" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B63" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C63" t="s">
         <v>15</v>
       </c>
       <c r="D63" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E63" t="s">
         <v>17</v>
@@ -3418,22 +3421,22 @@
         <v>21</v>
       </c>
       <c r="H63" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I63" t="s">
         <v>19</v>
       </c>
       <c r="J63" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K63" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L63" t="n">
         <v>0.391</v>
       </c>
       <c r="M63" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>